<commit_message>
Fixed FX Descriptive Stats
Run for BRL/TRY in line with Bberg CHECK excel.

Ran Rolling Stats and Correlations with new Descriptive Statistics function...

Leo: check is this makes sense.....
</commit_message>
<xml_diff>
--- a/DataOutPut/FX_Currencies_1-1-2008_12-31-2018.xlsx
+++ b/DataOutPut/FX_Currencies_1-1-2008_12-31-2018.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boris\LEM_Strategy\Software\Data_Download\DataOutPut\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0DB724-9B45-444D-BDFB-260E6BA5AAFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Corr" sheetId="2" r:id="rId2"/>
     <sheet name="CoVar" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,11 +45,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,13 +56,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,31 +95,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -182,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,27 +187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,24 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,16 +396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,50 +423,50 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>5.7247806728153003E-4</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9.6776625065251153E-3</v>
+      <c r="B2">
+        <v>0.00057247806728153</v>
+      </c>
+      <c r="C2">
+        <v>0.009677662506525115</v>
       </c>
       <c r="D2">
-        <v>9.3657151590201967E-5</v>
+        <v>9.365715159020197e-05</v>
       </c>
       <c r="E2">
-        <v>1.9141689194868909</v>
+        <v>1.914168919486891</v>
       </c>
       <c r="F2">
         <v>31.82353324928944</v>
       </c>
       <c r="G2">
-        <v>5.9154580653700162E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>0.05915458065370016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>3.4120416963180118E-4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.1019139406938621E-2</v>
+      <c r="B3">
+        <v>0.0003412041696318012</v>
+      </c>
+      <c r="C3">
+        <v>0.01101913940693862</v>
       </c>
       <c r="D3">
-        <v>1.2142143326954751E-4</v>
+        <v>0.0001214214332695475</v>
       </c>
       <c r="E3">
-        <v>0.32869616822344111</v>
+        <v>0.3286961682234411</v>
       </c>
       <c r="F3">
-        <v>5.3021750235841658</v>
+        <v>5.302175023584166</v>
       </c>
       <c r="G3">
-        <v>3.0964683994917901E-2</v>
+        <v>0.0309646839949179</v>
       </c>
     </row>
   </sheetData>
@@ -540,14 +475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -555,7 +490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -563,15 +498,15 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.45486196500275339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>0.4548619650027534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.45486196500275339</v>
+        <v>0.4548619650027534</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -583,14 +518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -598,26 +533,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>9.3657151590201967E-5</v>
+        <v>9.365715159020197e-05</v>
       </c>
       <c r="C2">
-        <v>4.9521327287268571E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>4.952132728726857e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>4.9521327287268571E-5</v>
+        <v>4.952132728726857e-05</v>
       </c>
       <c r="C3">
-        <v>1.2142143326954751E-4</v>
+        <v>0.0001214214332695475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>